<commit_message>
daily auto push: 2025-08-15 06:57 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2249"/>
+  <dimension ref="A1:D2250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40919,6 +40919,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2250">
+      <c r="A2250" t="inlineStr">
+        <is>
+          <t>2025/08/15</t>
+        </is>
+      </c>
+      <c r="B2250" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C2250" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2250" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-09-12 01:56 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2428"/>
+  <dimension ref="A1:D2429"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44141,6 +44141,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2429">
+      <c r="A2429" t="inlineStr">
+        <is>
+          <t>2025/09/12</t>
+        </is>
+      </c>
+      <c r="B2429" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C2429" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2429" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-10-09 02:00 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2561"/>
+  <dimension ref="A1:D2562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46535,6 +46535,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2562">
+      <c r="A2562" t="inlineStr">
+        <is>
+          <t>2025/10/09</t>
+        </is>
+      </c>
+      <c r="B2562" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C2562" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2562" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-11-04 09:33 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2682"/>
+  <dimension ref="A1:D2683"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48713,6 +48713,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2683">
+      <c r="A2683" t="inlineStr">
+        <is>
+          <t>2025/11/04</t>
+        </is>
+      </c>
+      <c r="B2683" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C2683" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2683" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-11-12 07:29 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2724"/>
+  <dimension ref="A1:D2725"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49469,6 +49469,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2725">
+      <c r="A2725" t="inlineStr">
+        <is>
+          <t>2025/11/12</t>
+        </is>
+      </c>
+      <c r="B2725" t="inlineStr">
+        <is>
+          <t>水</t>
+        </is>
+      </c>
+      <c r="C2725" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2725" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-11-30 07:27 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2815"/>
+  <dimension ref="A1:D2816"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51107,6 +51107,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2816">
+      <c r="A2816" t="inlineStr">
+        <is>
+          <t>2025/11/30</t>
+        </is>
+      </c>
+      <c r="B2816" t="inlineStr">
+        <is>
+          <t>日</t>
+        </is>
+      </c>
+      <c r="C2816" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2816" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-05 09:32 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2840"/>
+  <dimension ref="A1:D2841"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51557,6 +51557,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2841">
+      <c r="A2841" t="inlineStr">
+        <is>
+          <t>2025/12/05</t>
+        </is>
+      </c>
+      <c r="B2841" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C2841" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2841" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-11 09:36 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2869"/>
+  <dimension ref="A1:D2870"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52079,6 +52079,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2870">
+      <c r="A2870" t="inlineStr">
+        <is>
+          <t>2025/12/11</t>
+        </is>
+      </c>
+      <c r="B2870" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C2870" t="n">
+        <v>17</v>
+      </c>
+      <c r="D2870" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-25 03:42 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2956"/>
+  <dimension ref="A1:D2957"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53645,6 +53645,24 @@
         <v>201</v>
       </c>
     </row>
+    <row r="2957">
+      <c r="A2957" t="inlineStr">
+        <is>
+          <t>2025/12/25</t>
+        </is>
+      </c>
+      <c r="B2957" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C2957" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2957" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2026-01-05 13:49 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3086"/>
+  <dimension ref="A1:D3087"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55232,16 +55232,16 @@
     <row r="3045">
       <c r="A3045" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/05</t>
         </is>
       </c>
       <c r="B3045" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3045" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3045" t="n">
         <v>201</v>
@@ -55259,7 +55259,7 @@
         </is>
       </c>
       <c r="C3046" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3046" t="n">
         <v>201</v>
@@ -55277,7 +55277,7 @@
         </is>
       </c>
       <c r="C3047" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3047" t="n">
         <v>201</v>
@@ -55295,7 +55295,7 @@
         </is>
       </c>
       <c r="C3048" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3048" t="n">
         <v>201</v>
@@ -55304,16 +55304,16 @@
     <row r="3049">
       <c r="A3049" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3049" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3049" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3049" t="n">
         <v>201</v>
@@ -55331,7 +55331,7 @@
         </is>
       </c>
       <c r="C3050" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3050" t="n">
         <v>201</v>
@@ -55349,7 +55349,7 @@
         </is>
       </c>
       <c r="C3051" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3051" t="n">
         <v>201</v>
@@ -55367,7 +55367,7 @@
         </is>
       </c>
       <c r="C3052" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3052" t="n">
         <v>201</v>
@@ -55385,7 +55385,7 @@
         </is>
       </c>
       <c r="C3053" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3053" t="n">
         <v>201</v>
@@ -55403,7 +55403,7 @@
         </is>
       </c>
       <c r="C3054" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3054" t="n">
         <v>201</v>
@@ -55412,16 +55412,16 @@
     <row r="3055">
       <c r="A3055" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3055" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3055" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3055" t="n">
         <v>201</v>
@@ -55439,7 +55439,7 @@
         </is>
       </c>
       <c r="C3056" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3056" t="n">
         <v>201</v>
@@ -55457,7 +55457,7 @@
         </is>
       </c>
       <c r="C3057" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3057" t="n">
         <v>201</v>
@@ -55475,7 +55475,7 @@
         </is>
       </c>
       <c r="C3058" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3058" t="n">
         <v>201</v>
@@ -55493,7 +55493,7 @@
         </is>
       </c>
       <c r="C3059" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3059" t="n">
         <v>201</v>
@@ -55511,7 +55511,7 @@
         </is>
       </c>
       <c r="C3060" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3060" t="n">
         <v>201</v>
@@ -55520,16 +55520,16 @@
     <row r="3061">
       <c r="A3061" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3061" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3061" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3061" t="n">
         <v>201</v>
@@ -55547,7 +55547,7 @@
         </is>
       </c>
       <c r="C3062" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3062" t="n">
         <v>201</v>
@@ -55565,7 +55565,7 @@
         </is>
       </c>
       <c r="C3063" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3063" t="n">
         <v>201</v>
@@ -55583,7 +55583,7 @@
         </is>
       </c>
       <c r="C3064" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3064" t="n">
         <v>201</v>
@@ -55601,7 +55601,7 @@
         </is>
       </c>
       <c r="C3065" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3065" t="n">
         <v>201</v>
@@ -55610,16 +55610,16 @@
     <row r="3066">
       <c r="A3066" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3066" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3066" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3066" t="n">
         <v>201</v>
@@ -55637,7 +55637,7 @@
         </is>
       </c>
       <c r="C3067" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3067" t="n">
         <v>201</v>
@@ -55655,7 +55655,7 @@
         </is>
       </c>
       <c r="C3068" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3068" t="n">
         <v>201</v>
@@ -55673,7 +55673,7 @@
         </is>
       </c>
       <c r="C3069" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3069" t="n">
         <v>201</v>
@@ -55691,7 +55691,7 @@
         </is>
       </c>
       <c r="C3070" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3070" t="n">
         <v>201</v>
@@ -55709,7 +55709,7 @@
         </is>
       </c>
       <c r="C3071" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3071" t="n">
         <v>201</v>
@@ -55727,7 +55727,7 @@
         </is>
       </c>
       <c r="C3072" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3072" t="n">
         <v>201</v>
@@ -55736,16 +55736,16 @@
     <row r="3073">
       <c r="A3073" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3073" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3073" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3073" t="n">
         <v>201</v>
@@ -55763,7 +55763,7 @@
         </is>
       </c>
       <c r="C3074" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3074" t="n">
         <v>201</v>
@@ -55781,7 +55781,7 @@
         </is>
       </c>
       <c r="C3075" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3075" t="n">
         <v>201</v>
@@ -55799,7 +55799,7 @@
         </is>
       </c>
       <c r="C3076" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3076" t="n">
         <v>201</v>
@@ -55817,7 +55817,7 @@
         </is>
       </c>
       <c r="C3077" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3077" t="n">
         <v>201</v>
@@ -55835,7 +55835,7 @@
         </is>
       </c>
       <c r="C3078" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3078" t="n">
         <v>201</v>
@@ -55853,7 +55853,7 @@
         </is>
       </c>
       <c r="C3079" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3079" t="n">
         <v>201</v>
@@ -55862,16 +55862,16 @@
     <row r="3080">
       <c r="A3080" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3080" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3080" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3080" t="n">
         <v>201</v>
@@ -55889,7 +55889,7 @@
         </is>
       </c>
       <c r="C3081" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3081" t="n">
         <v>201</v>
@@ -55907,7 +55907,7 @@
         </is>
       </c>
       <c r="C3082" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3082" t="n">
         <v>201</v>
@@ -55925,7 +55925,7 @@
         </is>
       </c>
       <c r="C3083" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3083" t="n">
         <v>201</v>
@@ -55943,7 +55943,7 @@
         </is>
       </c>
       <c r="C3084" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3084" t="n">
         <v>201</v>
@@ -55952,16 +55952,16 @@
     <row r="3085">
       <c r="A3085" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3085" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3085" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3085" t="n">
         <v>201</v>
@@ -55979,9 +55979,27 @@
         </is>
       </c>
       <c r="C3086" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3086" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3087">
+      <c r="A3087" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3087" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3087" t="n">
         <v>7</v>
       </c>
-      <c r="D3086" t="n">
+      <c r="D3087" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-01-21 02:31 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3196"/>
+  <dimension ref="A1:D3198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57212,16 +57212,16 @@
     <row r="3155">
       <c r="A3155" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/21</t>
         </is>
       </c>
       <c r="B3155" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3155" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3155" t="n">
         <v>201</v>
@@ -57230,16 +57230,16 @@
     <row r="3156">
       <c r="A3156" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/21</t>
         </is>
       </c>
       <c r="B3156" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3156" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D3156" t="n">
         <v>201</v>
@@ -57257,7 +57257,7 @@
         </is>
       </c>
       <c r="C3157" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3157" t="n">
         <v>201</v>
@@ -57275,7 +57275,7 @@
         </is>
       </c>
       <c r="C3158" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D3158" t="n">
         <v>201</v>
@@ -57284,16 +57284,16 @@
     <row r="3159">
       <c r="A3159" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3159" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3159" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D3159" t="n">
         <v>201</v>
@@ -57302,16 +57302,16 @@
     <row r="3160">
       <c r="A3160" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3160" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3160" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D3160" t="n">
         <v>201</v>
@@ -57329,7 +57329,7 @@
         </is>
       </c>
       <c r="C3161" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3161" t="n">
         <v>201</v>
@@ -57347,7 +57347,7 @@
         </is>
       </c>
       <c r="C3162" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3162" t="n">
         <v>201</v>
@@ -57365,7 +57365,7 @@
         </is>
       </c>
       <c r="C3163" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3163" t="n">
         <v>201</v>
@@ -57383,7 +57383,7 @@
         </is>
       </c>
       <c r="C3164" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3164" t="n">
         <v>201</v>
@@ -57392,16 +57392,16 @@
     <row r="3165">
       <c r="A3165" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3165" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3165" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D3165" t="n">
         <v>201</v>
@@ -57410,16 +57410,16 @@
     <row r="3166">
       <c r="A3166" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3166" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3166" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D3166" t="n">
         <v>201</v>
@@ -57437,7 +57437,7 @@
         </is>
       </c>
       <c r="C3167" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3167" t="n">
         <v>201</v>
@@ -57455,7 +57455,7 @@
         </is>
       </c>
       <c r="C3168" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3168" t="n">
         <v>201</v>
@@ -57473,7 +57473,7 @@
         </is>
       </c>
       <c r="C3169" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3169" t="n">
         <v>201</v>
@@ -57491,7 +57491,7 @@
         </is>
       </c>
       <c r="C3170" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D3170" t="n">
         <v>201</v>
@@ -57500,16 +57500,16 @@
     <row r="3171">
       <c r="A3171" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3171" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3171" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3171" t="n">
         <v>201</v>
@@ -57518,16 +57518,16 @@
     <row r="3172">
       <c r="A3172" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3172" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3172" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D3172" t="n">
         <v>201</v>
@@ -57545,7 +57545,7 @@
         </is>
       </c>
       <c r="C3173" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D3173" t="n">
         <v>201</v>
@@ -57563,7 +57563,7 @@
         </is>
       </c>
       <c r="C3174" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D3174" t="n">
         <v>201</v>
@@ -57581,7 +57581,7 @@
         </is>
       </c>
       <c r="C3175" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3175" t="n">
         <v>201</v>
@@ -57590,16 +57590,16 @@
     <row r="3176">
       <c r="A3176" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3176" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3176" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D3176" t="n">
         <v>201</v>
@@ -57608,16 +57608,16 @@
     <row r="3177">
       <c r="A3177" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3177" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3177" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D3177" t="n">
         <v>201</v>
@@ -57635,7 +57635,7 @@
         </is>
       </c>
       <c r="C3178" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D3178" t="n">
         <v>201</v>
@@ -57653,7 +57653,7 @@
         </is>
       </c>
       <c r="C3179" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3179" t="n">
         <v>201</v>
@@ -57671,7 +57671,7 @@
         </is>
       </c>
       <c r="C3180" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3180" t="n">
         <v>201</v>
@@ -57689,7 +57689,7 @@
         </is>
       </c>
       <c r="C3181" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3181" t="n">
         <v>201</v>
@@ -57707,7 +57707,7 @@
         </is>
       </c>
       <c r="C3182" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3182" t="n">
         <v>201</v>
@@ -57716,16 +57716,16 @@
     <row r="3183">
       <c r="A3183" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3183" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3183" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3183" t="n">
         <v>201</v>
@@ -57734,16 +57734,16 @@
     <row r="3184">
       <c r="A3184" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3184" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3184" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3184" t="n">
         <v>201</v>
@@ -57761,7 +57761,7 @@
         </is>
       </c>
       <c r="C3185" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D3185" t="n">
         <v>201</v>
@@ -57779,7 +57779,7 @@
         </is>
       </c>
       <c r="C3186" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D3186" t="n">
         <v>201</v>
@@ -57797,7 +57797,7 @@
         </is>
       </c>
       <c r="C3187" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D3187" t="n">
         <v>201</v>
@@ -57815,7 +57815,7 @@
         </is>
       </c>
       <c r="C3188" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3188" t="n">
         <v>201</v>
@@ -57833,7 +57833,7 @@
         </is>
       </c>
       <c r="C3189" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3189" t="n">
         <v>201</v>
@@ -57842,16 +57842,16 @@
     <row r="3190">
       <c r="A3190" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3190" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3190" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D3190" t="n">
         <v>201</v>
@@ -57860,16 +57860,16 @@
     <row r="3191">
       <c r="A3191" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3191" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3191" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3191" t="n">
         <v>201</v>
@@ -57887,7 +57887,7 @@
         </is>
       </c>
       <c r="C3192" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3192" t="n">
         <v>201</v>
@@ -57905,7 +57905,7 @@
         </is>
       </c>
       <c r="C3193" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D3193" t="n">
         <v>201</v>
@@ -57923,7 +57923,7 @@
         </is>
       </c>
       <c r="C3194" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D3194" t="n">
         <v>201</v>
@@ -57932,16 +57932,16 @@
     <row r="3195">
       <c r="A3195" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3195" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3195" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D3195" t="n">
         <v>201</v>
@@ -57950,18 +57950,54 @@
     <row r="3196">
       <c r="A3196" t="inlineStr">
         <is>
+          <t>2027/01/04</t>
+        </is>
+      </c>
+      <c r="B3196" t="inlineStr">
+        <is>
+          <t>月</t>
+        </is>
+      </c>
+      <c r="C3196" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3196" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3197">
+      <c r="A3197" t="inlineStr">
+        <is>
           <t>2027/01/05</t>
         </is>
       </c>
-      <c r="B3196" t="inlineStr">
+      <c r="B3197" t="inlineStr">
         <is>
           <t>火</t>
         </is>
       </c>
-      <c r="C3196" t="n">
+      <c r="C3197" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3197" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3198">
+      <c r="A3198" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3198" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3198" t="n">
         <v>7</v>
       </c>
-      <c r="D3196" t="n">
+      <c r="D3198" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-01-23 22:33 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3215"/>
+  <dimension ref="A1:D3216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57554,16 +57554,16 @@
     <row r="3174">
       <c r="A3174" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/24</t>
         </is>
       </c>
       <c r="B3174" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3174" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D3174" t="n">
         <v>201</v>
@@ -57581,7 +57581,7 @@
         </is>
       </c>
       <c r="C3175" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3175" t="n">
         <v>201</v>
@@ -57599,7 +57599,7 @@
         </is>
       </c>
       <c r="C3176" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3176" t="n">
         <v>201</v>
@@ -57617,7 +57617,7 @@
         </is>
       </c>
       <c r="C3177" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3177" t="n">
         <v>201</v>
@@ -57626,16 +57626,16 @@
     <row r="3178">
       <c r="A3178" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3178" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3178" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3178" t="n">
         <v>201</v>
@@ -57653,7 +57653,7 @@
         </is>
       </c>
       <c r="C3179" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3179" t="n">
         <v>201</v>
@@ -57671,7 +57671,7 @@
         </is>
       </c>
       <c r="C3180" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3180" t="n">
         <v>201</v>
@@ -57689,7 +57689,7 @@
         </is>
       </c>
       <c r="C3181" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3181" t="n">
         <v>201</v>
@@ -57707,7 +57707,7 @@
         </is>
       </c>
       <c r="C3182" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3182" t="n">
         <v>201</v>
@@ -57725,7 +57725,7 @@
         </is>
       </c>
       <c r="C3183" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3183" t="n">
         <v>201</v>
@@ -57734,16 +57734,16 @@
     <row r="3184">
       <c r="A3184" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3184" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3184" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3184" t="n">
         <v>201</v>
@@ -57761,7 +57761,7 @@
         </is>
       </c>
       <c r="C3185" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3185" t="n">
         <v>201</v>
@@ -57779,7 +57779,7 @@
         </is>
       </c>
       <c r="C3186" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3186" t="n">
         <v>201</v>
@@ -57797,7 +57797,7 @@
         </is>
       </c>
       <c r="C3187" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3187" t="n">
         <v>201</v>
@@ -57815,7 +57815,7 @@
         </is>
       </c>
       <c r="C3188" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3188" t="n">
         <v>201</v>
@@ -57833,7 +57833,7 @@
         </is>
       </c>
       <c r="C3189" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3189" t="n">
         <v>201</v>
@@ -57842,16 +57842,16 @@
     <row r="3190">
       <c r="A3190" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3190" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3190" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3190" t="n">
         <v>201</v>
@@ -57869,7 +57869,7 @@
         </is>
       </c>
       <c r="C3191" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3191" t="n">
         <v>201</v>
@@ -57887,7 +57887,7 @@
         </is>
       </c>
       <c r="C3192" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3192" t="n">
         <v>201</v>
@@ -57905,7 +57905,7 @@
         </is>
       </c>
       <c r="C3193" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3193" t="n">
         <v>201</v>
@@ -57923,7 +57923,7 @@
         </is>
       </c>
       <c r="C3194" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3194" t="n">
         <v>201</v>
@@ -57932,16 +57932,16 @@
     <row r="3195">
       <c r="A3195" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3195" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3195" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3195" t="n">
         <v>201</v>
@@ -57959,7 +57959,7 @@
         </is>
       </c>
       <c r="C3196" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3196" t="n">
         <v>201</v>
@@ -57977,7 +57977,7 @@
         </is>
       </c>
       <c r="C3197" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3197" t="n">
         <v>201</v>
@@ -57995,7 +57995,7 @@
         </is>
       </c>
       <c r="C3198" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3198" t="n">
         <v>201</v>
@@ -58013,7 +58013,7 @@
         </is>
       </c>
       <c r="C3199" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3199" t="n">
         <v>201</v>
@@ -58031,7 +58031,7 @@
         </is>
       </c>
       <c r="C3200" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3200" t="n">
         <v>201</v>
@@ -58049,7 +58049,7 @@
         </is>
       </c>
       <c r="C3201" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3201" t="n">
         <v>201</v>
@@ -58058,16 +58058,16 @@
     <row r="3202">
       <c r="A3202" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3202" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3202" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3202" t="n">
         <v>201</v>
@@ -58085,7 +58085,7 @@
         </is>
       </c>
       <c r="C3203" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3203" t="n">
         <v>201</v>
@@ -58103,7 +58103,7 @@
         </is>
       </c>
       <c r="C3204" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3204" t="n">
         <v>201</v>
@@ -58121,7 +58121,7 @@
         </is>
       </c>
       <c r="C3205" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3205" t="n">
         <v>201</v>
@@ -58139,7 +58139,7 @@
         </is>
       </c>
       <c r="C3206" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3206" t="n">
         <v>201</v>
@@ -58157,7 +58157,7 @@
         </is>
       </c>
       <c r="C3207" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3207" t="n">
         <v>201</v>
@@ -58175,7 +58175,7 @@
         </is>
       </c>
       <c r="C3208" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3208" t="n">
         <v>201</v>
@@ -58184,16 +58184,16 @@
     <row r="3209">
       <c r="A3209" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3209" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3209" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3209" t="n">
         <v>201</v>
@@ -58211,7 +58211,7 @@
         </is>
       </c>
       <c r="C3210" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3210" t="n">
         <v>201</v>
@@ -58229,7 +58229,7 @@
         </is>
       </c>
       <c r="C3211" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3211" t="n">
         <v>201</v>
@@ -58247,7 +58247,7 @@
         </is>
       </c>
       <c r="C3212" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3212" t="n">
         <v>201</v>
@@ -58265,7 +58265,7 @@
         </is>
       </c>
       <c r="C3213" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3213" t="n">
         <v>201</v>
@@ -58274,16 +58274,16 @@
     <row r="3214">
       <c r="A3214" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3214" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3214" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3214" t="n">
         <v>201</v>
@@ -58301,9 +58301,27 @@
         </is>
       </c>
       <c r="C3215" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3215" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3216">
+      <c r="A3216" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3216" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3216" t="n">
         <v>7</v>
       </c>
-      <c r="D3215" t="n">
+      <c r="D3216" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-01-26 04:03 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3230"/>
+  <dimension ref="A1:D3231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57824,16 +57824,16 @@
     <row r="3189">
       <c r="A3189" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/26</t>
         </is>
       </c>
       <c r="B3189" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3189" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3189" t="n">
         <v>201</v>
@@ -57851,7 +57851,7 @@
         </is>
       </c>
       <c r="C3190" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3190" t="n">
         <v>201</v>
@@ -57869,7 +57869,7 @@
         </is>
       </c>
       <c r="C3191" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3191" t="n">
         <v>201</v>
@@ -57887,7 +57887,7 @@
         </is>
       </c>
       <c r="C3192" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3192" t="n">
         <v>201</v>
@@ -57896,16 +57896,16 @@
     <row r="3193">
       <c r="A3193" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3193" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3193" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3193" t="n">
         <v>201</v>
@@ -57923,7 +57923,7 @@
         </is>
       </c>
       <c r="C3194" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3194" t="n">
         <v>201</v>
@@ -57941,7 +57941,7 @@
         </is>
       </c>
       <c r="C3195" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3195" t="n">
         <v>201</v>
@@ -57959,7 +57959,7 @@
         </is>
       </c>
       <c r="C3196" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3196" t="n">
         <v>201</v>
@@ -57977,7 +57977,7 @@
         </is>
       </c>
       <c r="C3197" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3197" t="n">
         <v>201</v>
@@ -57995,7 +57995,7 @@
         </is>
       </c>
       <c r="C3198" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3198" t="n">
         <v>201</v>
@@ -58004,16 +58004,16 @@
     <row r="3199">
       <c r="A3199" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3199" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3199" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3199" t="n">
         <v>201</v>
@@ -58031,7 +58031,7 @@
         </is>
       </c>
       <c r="C3200" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3200" t="n">
         <v>201</v>
@@ -58049,7 +58049,7 @@
         </is>
       </c>
       <c r="C3201" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3201" t="n">
         <v>201</v>
@@ -58067,7 +58067,7 @@
         </is>
       </c>
       <c r="C3202" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3202" t="n">
         <v>201</v>
@@ -58085,7 +58085,7 @@
         </is>
       </c>
       <c r="C3203" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3203" t="n">
         <v>201</v>
@@ -58103,7 +58103,7 @@
         </is>
       </c>
       <c r="C3204" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3204" t="n">
         <v>201</v>
@@ -58112,16 +58112,16 @@
     <row r="3205">
       <c r="A3205" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3205" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3205" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3205" t="n">
         <v>201</v>
@@ -58139,7 +58139,7 @@
         </is>
       </c>
       <c r="C3206" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3206" t="n">
         <v>201</v>
@@ -58157,7 +58157,7 @@
         </is>
       </c>
       <c r="C3207" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3207" t="n">
         <v>201</v>
@@ -58175,7 +58175,7 @@
         </is>
       </c>
       <c r="C3208" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3208" t="n">
         <v>201</v>
@@ -58193,7 +58193,7 @@
         </is>
       </c>
       <c r="C3209" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3209" t="n">
         <v>201</v>
@@ -58202,16 +58202,16 @@
     <row r="3210">
       <c r="A3210" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3210" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3210" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3210" t="n">
         <v>201</v>
@@ -58229,7 +58229,7 @@
         </is>
       </c>
       <c r="C3211" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3211" t="n">
         <v>201</v>
@@ -58247,7 +58247,7 @@
         </is>
       </c>
       <c r="C3212" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3212" t="n">
         <v>201</v>
@@ -58265,7 +58265,7 @@
         </is>
       </c>
       <c r="C3213" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3213" t="n">
         <v>201</v>
@@ -58283,7 +58283,7 @@
         </is>
       </c>
       <c r="C3214" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3214" t="n">
         <v>201</v>
@@ -58301,7 +58301,7 @@
         </is>
       </c>
       <c r="C3215" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3215" t="n">
         <v>201</v>
@@ -58319,7 +58319,7 @@
         </is>
       </c>
       <c r="C3216" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3216" t="n">
         <v>201</v>
@@ -58328,16 +58328,16 @@
     <row r="3217">
       <c r="A3217" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3217" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3217" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3217" t="n">
         <v>201</v>
@@ -58355,7 +58355,7 @@
         </is>
       </c>
       <c r="C3218" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3218" t="n">
         <v>201</v>
@@ -58373,7 +58373,7 @@
         </is>
       </c>
       <c r="C3219" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3219" t="n">
         <v>201</v>
@@ -58391,7 +58391,7 @@
         </is>
       </c>
       <c r="C3220" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3220" t="n">
         <v>201</v>
@@ -58409,7 +58409,7 @@
         </is>
       </c>
       <c r="C3221" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3221" t="n">
         <v>201</v>
@@ -58427,7 +58427,7 @@
         </is>
       </c>
       <c r="C3222" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3222" t="n">
         <v>201</v>
@@ -58445,7 +58445,7 @@
         </is>
       </c>
       <c r="C3223" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3223" t="n">
         <v>201</v>
@@ -58454,16 +58454,16 @@
     <row r="3224">
       <c r="A3224" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3224" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3224" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3224" t="n">
         <v>201</v>
@@ -58481,7 +58481,7 @@
         </is>
       </c>
       <c r="C3225" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3225" t="n">
         <v>201</v>
@@ -58499,7 +58499,7 @@
         </is>
       </c>
       <c r="C3226" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3226" t="n">
         <v>201</v>
@@ -58517,7 +58517,7 @@
         </is>
       </c>
       <c r="C3227" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3227" t="n">
         <v>201</v>
@@ -58535,7 +58535,7 @@
         </is>
       </c>
       <c r="C3228" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3228" t="n">
         <v>201</v>
@@ -58544,16 +58544,16 @@
     <row r="3229">
       <c r="A3229" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3229" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3229" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3229" t="n">
         <v>201</v>
@@ -58571,9 +58571,27 @@
         </is>
       </c>
       <c r="C3230" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3230" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3231">
+      <c r="A3231" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3231" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3231" t="n">
         <v>7</v>
       </c>
-      <c r="D3230" t="n">
+      <c r="D3231" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-01-28 22:45 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3245"/>
+  <dimension ref="A1:D3247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58094,16 +58094,16 @@
     <row r="3204">
       <c r="A3204" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/29</t>
         </is>
       </c>
       <c r="B3204" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3204" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D3204" t="n">
         <v>201</v>
@@ -58112,16 +58112,16 @@
     <row r="3205">
       <c r="A3205" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/29</t>
         </is>
       </c>
       <c r="B3205" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3205" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D3205" t="n">
         <v>201</v>
@@ -58139,7 +58139,7 @@
         </is>
       </c>
       <c r="C3206" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3206" t="n">
         <v>201</v>
@@ -58157,7 +58157,7 @@
         </is>
       </c>
       <c r="C3207" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D3207" t="n">
         <v>201</v>
@@ -58166,16 +58166,16 @@
     <row r="3208">
       <c r="A3208" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3208" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3208" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D3208" t="n">
         <v>201</v>
@@ -58184,16 +58184,16 @@
     <row r="3209">
       <c r="A3209" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3209" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3209" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D3209" t="n">
         <v>201</v>
@@ -58211,7 +58211,7 @@
         </is>
       </c>
       <c r="C3210" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3210" t="n">
         <v>201</v>
@@ -58229,7 +58229,7 @@
         </is>
       </c>
       <c r="C3211" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3211" t="n">
         <v>201</v>
@@ -58247,7 +58247,7 @@
         </is>
       </c>
       <c r="C3212" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3212" t="n">
         <v>201</v>
@@ -58265,7 +58265,7 @@
         </is>
       </c>
       <c r="C3213" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3213" t="n">
         <v>201</v>
@@ -58274,16 +58274,16 @@
     <row r="3214">
       <c r="A3214" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3214" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3214" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D3214" t="n">
         <v>201</v>
@@ -58292,16 +58292,16 @@
     <row r="3215">
       <c r="A3215" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3215" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3215" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D3215" t="n">
         <v>201</v>
@@ -58319,7 +58319,7 @@
         </is>
       </c>
       <c r="C3216" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3216" t="n">
         <v>201</v>
@@ -58337,7 +58337,7 @@
         </is>
       </c>
       <c r="C3217" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3217" t="n">
         <v>201</v>
@@ -58355,7 +58355,7 @@
         </is>
       </c>
       <c r="C3218" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3218" t="n">
         <v>201</v>
@@ -58373,7 +58373,7 @@
         </is>
       </c>
       <c r="C3219" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D3219" t="n">
         <v>201</v>
@@ -58382,16 +58382,16 @@
     <row r="3220">
       <c r="A3220" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3220" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3220" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3220" t="n">
         <v>201</v>
@@ -58400,16 +58400,16 @@
     <row r="3221">
       <c r="A3221" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3221" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3221" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D3221" t="n">
         <v>201</v>
@@ -58427,7 +58427,7 @@
         </is>
       </c>
       <c r="C3222" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D3222" t="n">
         <v>201</v>
@@ -58445,7 +58445,7 @@
         </is>
       </c>
       <c r="C3223" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D3223" t="n">
         <v>201</v>
@@ -58463,7 +58463,7 @@
         </is>
       </c>
       <c r="C3224" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3224" t="n">
         <v>201</v>
@@ -58472,16 +58472,16 @@
     <row r="3225">
       <c r="A3225" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3225" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3225" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D3225" t="n">
         <v>201</v>
@@ -58490,16 +58490,16 @@
     <row r="3226">
       <c r="A3226" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3226" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3226" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D3226" t="n">
         <v>201</v>
@@ -58517,7 +58517,7 @@
         </is>
       </c>
       <c r="C3227" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D3227" t="n">
         <v>201</v>
@@ -58535,7 +58535,7 @@
         </is>
       </c>
       <c r="C3228" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3228" t="n">
         <v>201</v>
@@ -58553,7 +58553,7 @@
         </is>
       </c>
       <c r="C3229" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3229" t="n">
         <v>201</v>
@@ -58571,7 +58571,7 @@
         </is>
       </c>
       <c r="C3230" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3230" t="n">
         <v>201</v>
@@ -58589,7 +58589,7 @@
         </is>
       </c>
       <c r="C3231" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3231" t="n">
         <v>201</v>
@@ -58598,16 +58598,16 @@
     <row r="3232">
       <c r="A3232" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3232" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3232" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3232" t="n">
         <v>201</v>
@@ -58616,16 +58616,16 @@
     <row r="3233">
       <c r="A3233" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3233" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3233" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3233" t="n">
         <v>201</v>
@@ -58643,7 +58643,7 @@
         </is>
       </c>
       <c r="C3234" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D3234" t="n">
         <v>201</v>
@@ -58661,7 +58661,7 @@
         </is>
       </c>
       <c r="C3235" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D3235" t="n">
         <v>201</v>
@@ -58679,7 +58679,7 @@
         </is>
       </c>
       <c r="C3236" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D3236" t="n">
         <v>201</v>
@@ -58697,7 +58697,7 @@
         </is>
       </c>
       <c r="C3237" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3237" t="n">
         <v>201</v>
@@ -58715,7 +58715,7 @@
         </is>
       </c>
       <c r="C3238" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3238" t="n">
         <v>201</v>
@@ -58724,16 +58724,16 @@
     <row r="3239">
       <c r="A3239" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3239" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3239" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D3239" t="n">
         <v>201</v>
@@ -58742,16 +58742,16 @@
     <row r="3240">
       <c r="A3240" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3240" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3240" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3240" t="n">
         <v>201</v>
@@ -58769,7 +58769,7 @@
         </is>
       </c>
       <c r="C3241" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3241" t="n">
         <v>201</v>
@@ -58787,7 +58787,7 @@
         </is>
       </c>
       <c r="C3242" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D3242" t="n">
         <v>201</v>
@@ -58805,7 +58805,7 @@
         </is>
       </c>
       <c r="C3243" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D3243" t="n">
         <v>201</v>
@@ -58814,16 +58814,16 @@
     <row r="3244">
       <c r="A3244" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3244" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3244" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D3244" t="n">
         <v>201</v>
@@ -58832,18 +58832,54 @@
     <row r="3245">
       <c r="A3245" t="inlineStr">
         <is>
+          <t>2027/01/04</t>
+        </is>
+      </c>
+      <c r="B3245" t="inlineStr">
+        <is>
+          <t>月</t>
+        </is>
+      </c>
+      <c r="C3245" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3245" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3246">
+      <c r="A3246" t="inlineStr">
+        <is>
           <t>2027/01/05</t>
         </is>
       </c>
-      <c r="B3245" t="inlineStr">
+      <c r="B3246" t="inlineStr">
         <is>
           <t>火</t>
         </is>
       </c>
-      <c r="C3245" t="n">
+      <c r="C3246" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3246" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3247">
+      <c r="A3247" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3247" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3247" t="n">
         <v>7</v>
       </c>
-      <c r="D3245" t="n">
+      <c r="D3247" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-01-29 09:56 UTC
</commit_message>
<xml_diff>
--- a/excel/apple2.xlsx
+++ b/excel/apple2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3249"/>
+  <dimension ref="A1:D3250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58166,16 +58166,16 @@
     <row r="3208">
       <c r="A3208" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/29</t>
         </is>
       </c>
       <c r="B3208" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3208" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3208" t="n">
         <v>201</v>
@@ -58193,7 +58193,7 @@
         </is>
       </c>
       <c r="C3209" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3209" t="n">
         <v>201</v>
@@ -58211,7 +58211,7 @@
         </is>
       </c>
       <c r="C3210" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3210" t="n">
         <v>201</v>
@@ -58229,7 +58229,7 @@
         </is>
       </c>
       <c r="C3211" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3211" t="n">
         <v>201</v>
@@ -58238,16 +58238,16 @@
     <row r="3212">
       <c r="A3212" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3212" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3212" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3212" t="n">
         <v>201</v>
@@ -58265,7 +58265,7 @@
         </is>
       </c>
       <c r="C3213" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3213" t="n">
         <v>201</v>
@@ -58283,7 +58283,7 @@
         </is>
       </c>
       <c r="C3214" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3214" t="n">
         <v>201</v>
@@ -58301,7 +58301,7 @@
         </is>
       </c>
       <c r="C3215" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3215" t="n">
         <v>201</v>
@@ -58319,7 +58319,7 @@
         </is>
       </c>
       <c r="C3216" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3216" t="n">
         <v>201</v>
@@ -58337,7 +58337,7 @@
         </is>
       </c>
       <c r="C3217" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3217" t="n">
         <v>201</v>
@@ -58346,16 +58346,16 @@
     <row r="3218">
       <c r="A3218" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3218" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3218" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3218" t="n">
         <v>201</v>
@@ -58373,7 +58373,7 @@
         </is>
       </c>
       <c r="C3219" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3219" t="n">
         <v>201</v>
@@ -58391,7 +58391,7 @@
         </is>
       </c>
       <c r="C3220" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3220" t="n">
         <v>201</v>
@@ -58409,7 +58409,7 @@
         </is>
       </c>
       <c r="C3221" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3221" t="n">
         <v>201</v>
@@ -58427,7 +58427,7 @@
         </is>
       </c>
       <c r="C3222" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3222" t="n">
         <v>201</v>
@@ -58445,7 +58445,7 @@
         </is>
       </c>
       <c r="C3223" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3223" t="n">
         <v>201</v>
@@ -58454,16 +58454,16 @@
     <row r="3224">
       <c r="A3224" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3224" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3224" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3224" t="n">
         <v>201</v>
@@ -58481,7 +58481,7 @@
         </is>
       </c>
       <c r="C3225" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3225" t="n">
         <v>201</v>
@@ -58499,7 +58499,7 @@
         </is>
       </c>
       <c r="C3226" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3226" t="n">
         <v>201</v>
@@ -58517,7 +58517,7 @@
         </is>
       </c>
       <c r="C3227" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3227" t="n">
         <v>201</v>
@@ -58535,7 +58535,7 @@
         </is>
       </c>
       <c r="C3228" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3228" t="n">
         <v>201</v>
@@ -58544,16 +58544,16 @@
     <row r="3229">
       <c r="A3229" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3229" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3229" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3229" t="n">
         <v>201</v>
@@ -58571,7 +58571,7 @@
         </is>
       </c>
       <c r="C3230" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3230" t="n">
         <v>201</v>
@@ -58589,7 +58589,7 @@
         </is>
       </c>
       <c r="C3231" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3231" t="n">
         <v>201</v>
@@ -58607,7 +58607,7 @@
         </is>
       </c>
       <c r="C3232" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3232" t="n">
         <v>201</v>
@@ -58625,7 +58625,7 @@
         </is>
       </c>
       <c r="C3233" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3233" t="n">
         <v>201</v>
@@ -58643,7 +58643,7 @@
         </is>
       </c>
       <c r="C3234" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3234" t="n">
         <v>201</v>
@@ -58661,7 +58661,7 @@
         </is>
       </c>
       <c r="C3235" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3235" t="n">
         <v>201</v>
@@ -58670,16 +58670,16 @@
     <row r="3236">
       <c r="A3236" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3236" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3236" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3236" t="n">
         <v>201</v>
@@ -58697,7 +58697,7 @@
         </is>
       </c>
       <c r="C3237" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3237" t="n">
         <v>201</v>
@@ -58715,7 +58715,7 @@
         </is>
       </c>
       <c r="C3238" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3238" t="n">
         <v>201</v>
@@ -58733,7 +58733,7 @@
         </is>
       </c>
       <c r="C3239" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3239" t="n">
         <v>201</v>
@@ -58751,7 +58751,7 @@
         </is>
       </c>
       <c r="C3240" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3240" t="n">
         <v>201</v>
@@ -58769,7 +58769,7 @@
         </is>
       </c>
       <c r="C3241" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3241" t="n">
         <v>201</v>
@@ -58787,7 +58787,7 @@
         </is>
       </c>
       <c r="C3242" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3242" t="n">
         <v>201</v>
@@ -58796,16 +58796,16 @@
     <row r="3243">
       <c r="A3243" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3243" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3243" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3243" t="n">
         <v>201</v>
@@ -58823,7 +58823,7 @@
         </is>
       </c>
       <c r="C3244" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3244" t="n">
         <v>201</v>
@@ -58841,7 +58841,7 @@
         </is>
       </c>
       <c r="C3245" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3245" t="n">
         <v>201</v>
@@ -58859,7 +58859,7 @@
         </is>
       </c>
       <c r="C3246" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3246" t="n">
         <v>201</v>
@@ -58877,7 +58877,7 @@
         </is>
       </c>
       <c r="C3247" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3247" t="n">
         <v>201</v>
@@ -58886,16 +58886,16 @@
     <row r="3248">
       <c r="A3248" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3248" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3248" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3248" t="n">
         <v>201</v>
@@ -58913,9 +58913,27 @@
         </is>
       </c>
       <c r="C3249" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3249" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3250">
+      <c r="A3250" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3250" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3250" t="n">
         <v>7</v>
       </c>
-      <c r="D3249" t="n">
+      <c r="D3250" t="n">
         <v>201</v>
       </c>
     </row>

</xml_diff>